<commit_message>
fine tuning jira REST API
</commit_message>
<xml_diff>
--- a/Worklog Entry Template.xlsx
+++ b/Worklog Entry Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rApiiNel\Documents\personal_projects\jira_worklog_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81321CE4-DD7C-4382-B6B4-7DA6D24B8A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB2A5D4-0D1B-414A-8F0A-664148FBDD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,23 +32,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15268" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15243" uniqueCount="845">
   <si>
     <t>Team</t>
   </si>
@@ -2583,21 +2572,6 @@
   </si>
   <si>
     <t>Test 2</t>
-  </si>
-  <si>
-    <t>Test 3</t>
-  </si>
-  <si>
-    <t>Test 4</t>
-  </si>
-  <si>
-    <t>Test 5</t>
-  </si>
-  <si>
-    <t>Test 6</t>
-  </si>
-  <si>
-    <t>Test 7</t>
   </si>
 </sst>
 </file>
@@ -4013,10 +3987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -4100,121 +4074,6 @@
         <v>844</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="205">
-        <v>44911</v>
-      </c>
-      <c r="B4" s="206" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="207" t="s">
-        <v>842</v>
-      </c>
-      <c r="E4" s="208" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="209">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="208" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="205">
-        <v>44911</v>
-      </c>
-      <c r="B5" s="206" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="207" t="s">
-        <v>842</v>
-      </c>
-      <c r="E5" s="208" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="209">
-        <v>1.5</v>
-      </c>
-      <c r="G5" s="208" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="205">
-        <v>44911</v>
-      </c>
-      <c r="B6" s="206" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="207" t="s">
-        <v>842</v>
-      </c>
-      <c r="E6" s="208" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="209">
-        <v>1</v>
-      </c>
-      <c r="G6" s="208" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="205">
-        <v>44911</v>
-      </c>
-      <c r="B7" s="206" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="207" t="s">
-        <v>842</v>
-      </c>
-      <c r="E7" s="208" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="209">
-        <v>1</v>
-      </c>
-      <c r="G7" s="208" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="205">
-        <v>44911</v>
-      </c>
-      <c r="B8" s="206" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="207" t="s">
-        <v>842</v>
-      </c>
-      <c r="E8" s="208" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="209">
-        <v>3</v>
-      </c>
-      <c r="G8" s="208" t="s">
-        <v>849</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="25" type="noConversion"/>
@@ -4222,13 +4081,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1 B9:B1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1 B4:B1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{0FCE1531-446D-4DF3-B797-BAFB6B0CD871}"/>
-    <hyperlink ref="D3:D8" r:id="rId2" display="https://legalmatch.atlassian.net/browse/SAL-500" xr:uid="{3A54D241-98B8-4AE3-B4DF-DE3CFC9FCC5F}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{3A54D241-98B8-4AE3-B4DF-DE3CFC9FCC5F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -76256,6 +76115,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="472e3545-f2f9-45a4-a835-21f36fafbe41" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a3da683f-a0db-4096-acd9-53a5b471ce97">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004CA055D7B43CB7419EB33CE46DECFB6B" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="45e5190158379cbed2e72a24731d3f02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a3da683f-a0db-4096-acd9-53a5b471ce97" xmlns:ns3="472e3545-f2f9-45a4-a835-21f36fafbe41" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8abf491b97c7162b5ed8f2adfd2a5616" ns2:_="" ns3:_="">
     <xsd:import namespace="a3da683f-a0db-4096-acd9-53a5b471ce97"/>
@@ -76498,17 +76368,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="472e3545-f2f9-45a4-a835-21f36fafbe41" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a3da683f-a0db-4096-acd9-53a5b471ce97">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -76519,6 +76378,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D58BA3B-EDE5-4159-BAB5-B0762F6AA8CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="472e3545-f2f9-45a4-a835-21f36fafbe41"/>
+    <ds:schemaRef ds:uri="a3da683f-a0db-4096-acd9-53a5b471ce97"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2CC3277-B46B-475B-A1E0-559D08A06A52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -76537,17 +76407,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D58BA3B-EDE5-4159-BAB5-B0762F6AA8CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="472e3545-f2f9-45a4-a835-21f36fafbe41"/>
-    <ds:schemaRef ds:uri="a3da683f-a0db-4096-acd9-53a5b471ce97"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E483523F-ABFE-46F1-A03B-718B74E234A9}">
   <ds:schemaRefs>

</xml_diff>